<commit_message>
Added Chapter-by-Chapter and Overall Progress Statistics to the progress tracker
</commit_message>
<xml_diff>
--- a/Principles of Mathematical Analysis - Progress.xlsx
+++ b/Principles of Mathematical Analysis - Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TeX\Books\Rudin, Walter\Principles of Mathematical Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4DDF13-A521-47D2-BDA0-65826ACB91E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753DF579-FB83-44B2-BB08-996E2DCF3B6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4ECAD2DA-16DF-447C-94EF-7D164C966ED4}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ProblemsStatus">Main!$D$2:$D$31,Main!$F$2:$F$26,Main!$H$2:$H$27,Main!$B$2:$B$21,Main!$J$2:$J$30,Main!$L$2:$L$20,Main!$N$2:$N$27,Main!$P$2:$P$32,Main!$R$2:$R$32,Main!$T$2:$T$33,Main!$V$2:$V$19</definedName>
+    <definedName name="ProblemsStatus">Main!$E$2:$E$31,Main!$G$2:$G$26,Main!$I$2:$I$27,Main!$C$2:$C$21,Main!$K$2:$K$30,Main!$M$2:$M$20,Main!$O$2:$O$27,Main!$Q$2:$Q$32,Main!$S$2:$S$32,Main!$U$2:$U$33,Main!$W$2:$W$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
   <si>
     <t>Status</t>
   </si>
@@ -80,12 +80,28 @@
   <si>
     <t>Chapter 11</t>
   </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>Problems</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,10 +127,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -122,11 +139,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="4">
     <dxf>
       <font>
         <strike val="0"/>
@@ -156,17 +178,6 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
           <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
@@ -498,1340 +509,1632 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EB77106-B98B-4FF2-B67C-6A4D8C99C21E}">
-  <dimension ref="A1:V33"/>
+  <dimension ref="A1:Y39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="3.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="3.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="3.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="3.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="3.42578125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="3.42578125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="13.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="3.42578125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="3.42578125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="13.7109375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="3.42578125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="13.7109375" style="1" customWidth="1"/>
-    <col min="21" max="21" width="3.42578125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="13.7109375" style="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="3.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="3.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="3.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="3.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="3.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="3.42578125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="3.42578125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="3.42578125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="3.42578125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="13.7109375" style="1" customWidth="1"/>
+    <col min="22" max="22" width="3.42578125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="13.7109375" style="1" customWidth="1"/>
+    <col min="24" max="24" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="2"/>
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="2"/>
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="2"/>
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="2"/>
+      <c r="L1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="2"/>
+      <c r="N1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="2"/>
+      <c r="P1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="2"/>
+      <c r="T1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="2"/>
+      <c r="V1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="V1" s="2"/>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="W1" s="2"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+    </row>
+    <row r="2" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1">
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="1">
+      <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1">
         <v>1</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="1">
+      <c r="G2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="1">
         <v>1</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="1">
+      <c r="J2" s="1">
         <v>1</v>
       </c>
-      <c r="K2" s="1">
+      <c r="L2" s="1">
         <v>1</v>
       </c>
-      <c r="M2" s="1">
+      <c r="N2" s="1">
         <v>1</v>
       </c>
-      <c r="O2" s="1">
+      <c r="P2" s="1">
         <v>1</v>
       </c>
-      <c r="Q2" s="1">
+      <c r="R2" s="1">
         <v>1</v>
       </c>
-      <c r="S2" s="1">
+      <c r="T2" s="1">
         <v>1</v>
       </c>
-      <c r="U2" s="1">
+      <c r="V2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <f>A2+1</f>
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1">
-        <f>C2+1</f>
-        <v>2</v>
-      </c>
-      <c r="E3" s="1">
-        <f>E2+1</f>
-        <v>2</v>
-      </c>
-      <c r="G3" s="1">
-        <f>G2+1</f>
-        <v>2</v>
-      </c>
-      <c r="I3" s="1">
-        <f>I2+1</f>
-        <v>2</v>
-      </c>
-      <c r="K3" s="1">
-        <f>K2+1</f>
-        <v>2</v>
-      </c>
-      <c r="M3" s="1">
-        <f>M2+1</f>
-        <v>2</v>
-      </c>
-      <c r="O3" s="1">
-        <f>O2+1</f>
-        <v>2</v>
-      </c>
-      <c r="Q3" s="1">
-        <f>Q2+1</f>
-        <v>2</v>
-      </c>
-      <c r="S3" s="1">
-        <f>S2+1</f>
-        <v>2</v>
-      </c>
-      <c r="U3" s="1">
-        <f>U2+1</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <f t="shared" ref="A4:A22" si="0">A3+1</f>
+    <row r="3" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
+        <f>B2+1</f>
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
+        <f>D2+1</f>
+        <v>2</v>
+      </c>
+      <c r="F3" s="1">
+        <f>F2+1</f>
+        <v>2</v>
+      </c>
+      <c r="H3" s="1">
+        <f>H2+1</f>
+        <v>2</v>
+      </c>
+      <c r="J3" s="1">
+        <f>J2+1</f>
+        <v>2</v>
+      </c>
+      <c r="L3" s="1">
+        <f>L2+1</f>
+        <v>2</v>
+      </c>
+      <c r="N3" s="1">
+        <f>N2+1</f>
+        <v>2</v>
+      </c>
+      <c r="P3" s="1">
+        <f>P2+1</f>
+        <v>2</v>
+      </c>
+      <c r="R3" s="1">
+        <f>R2+1</f>
+        <v>2</v>
+      </c>
+      <c r="T3" s="1">
+        <f>T2+1</f>
+        <v>2</v>
+      </c>
+      <c r="V3" s="1">
+        <f>V2+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <f t="shared" ref="B4:B21" si="0">B3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1">
-        <f t="shared" ref="C4:C30" si="1">C3+1</f>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" ref="D4:D30" si="1">D3+1</f>
         <v>3</v>
       </c>
-      <c r="E4" s="1">
-        <f t="shared" ref="E4:E26" si="2">E3+1</f>
+      <c r="F4" s="1">
+        <f t="shared" ref="F4:F26" si="2">F3+1</f>
         <v>3</v>
       </c>
-      <c r="G4" s="1">
-        <f t="shared" ref="G4:G27" si="3">G3+1</f>
+      <c r="H4" s="1">
+        <f t="shared" ref="H4:H27" si="3">H3+1</f>
         <v>3</v>
       </c>
-      <c r="I4" s="1">
-        <f t="shared" ref="I4:I30" si="4">I3+1</f>
+      <c r="J4" s="1">
+        <f t="shared" ref="J4:J30" si="4">J3+1</f>
         <v>3</v>
       </c>
-      <c r="K4" s="1">
-        <f t="shared" ref="K4:K20" si="5">K3+1</f>
+      <c r="L4" s="1">
+        <f t="shared" ref="L4:L20" si="5">L3+1</f>
         <v>3</v>
       </c>
-      <c r="M4" s="1">
-        <f t="shared" ref="M4:M27" si="6">M3+1</f>
+      <c r="N4" s="1">
+        <f t="shared" ref="N4:N27" si="6">N3+1</f>
         <v>3</v>
       </c>
-      <c r="O4" s="1">
-        <f t="shared" ref="O4:O32" si="7">O3+1</f>
+      <c r="P4" s="1">
+        <f t="shared" ref="P4:P32" si="7">P3+1</f>
         <v>3</v>
       </c>
-      <c r="Q4" s="1">
-        <f t="shared" ref="Q4:Q32" si="8">Q3+1</f>
+      <c r="R4" s="1">
+        <f t="shared" ref="R4:R32" si="8">R3+1</f>
         <v>3</v>
       </c>
-      <c r="S4" s="1">
-        <f t="shared" ref="S4:S33" si="9">S3+1</f>
+      <c r="T4" s="1">
+        <f t="shared" ref="T4:T33" si="9">T3+1</f>
         <v>3</v>
       </c>
-      <c r="U4" s="1">
-        <f t="shared" ref="U4:U19" si="10">U3+1</f>
+      <c r="V4" s="1">
+        <f t="shared" ref="V4:V19" si="10">V3+1</f>
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    <row r="5" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1">
+      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="1">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="1">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="K5" s="1">
+      <c r="L5" s="1">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="M5" s="1">
+      <c r="N5" s="1">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="O5" s="1">
+      <c r="P5" s="1">
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
-      <c r="Q5" s="1">
+      <c r="R5" s="1">
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="S5" s="1">
+      <c r="T5" s="1">
         <f t="shared" si="9"/>
         <v>4</v>
       </c>
-      <c r="U5" s="1">
+      <c r="V5" s="1">
         <f t="shared" si="10"/>
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="6" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="1">
+      <c r="C6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J6" s="1">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="K6" s="1">
+      <c r="L6" s="1">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="M6" s="1">
+      <c r="N6" s="1">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
-      <c r="O6" s="1">
+      <c r="P6" s="1">
         <f t="shared" si="7"/>
         <v>5</v>
       </c>
-      <c r="Q6" s="1">
+      <c r="R6" s="1">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="S6" s="1">
+      <c r="T6" s="1">
         <f t="shared" si="9"/>
         <v>5</v>
       </c>
-      <c r="U6" s="1">
+      <c r="V6" s="1">
         <f t="shared" si="10"/>
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    <row r="7" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="K7" s="1">
+      <c r="L7" s="1">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="M7" s="1">
+      <c r="N7" s="1">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
-      <c r="O7" s="1">
+      <c r="P7" s="1">
         <f t="shared" si="7"/>
         <v>6</v>
       </c>
-      <c r="Q7" s="1">
+      <c r="R7" s="1">
         <f t="shared" si="8"/>
         <v>6</v>
       </c>
-      <c r="S7" s="1">
+      <c r="T7" s="1">
         <f t="shared" si="9"/>
         <v>6</v>
       </c>
-      <c r="U7" s="1">
+      <c r="V7" s="1">
         <f t="shared" si="10"/>
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+    <row r="8" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="1">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H8" s="1">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="I8" s="1">
+      <c r="J8" s="1">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="K8" s="1">
+      <c r="L8" s="1">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="M8" s="1">
+      <c r="N8" s="1">
         <f t="shared" si="6"/>
         <v>7</v>
       </c>
-      <c r="O8" s="1">
+      <c r="P8" s="1">
         <f t="shared" si="7"/>
         <v>7</v>
       </c>
-      <c r="Q8" s="1">
+      <c r="R8" s="1">
         <f t="shared" si="8"/>
         <v>7</v>
       </c>
-      <c r="S8" s="1">
+      <c r="T8" s="1">
         <f t="shared" si="9"/>
         <v>7</v>
       </c>
-      <c r="U8" s="1">
+      <c r="V8" s="1">
         <f t="shared" si="10"/>
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+    <row r="9" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C9" s="1">
+      <c r="D9" s="1">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="G9" s="1">
+      <c r="H9" s="1">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="I9" s="1">
+      <c r="J9" s="1">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="K9" s="1">
+      <c r="L9" s="1">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="M9" s="1">
+      <c r="N9" s="1">
         <f t="shared" si="6"/>
         <v>8</v>
       </c>
-      <c r="O9" s="1">
+      <c r="P9" s="1">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="Q9" s="1">
+      <c r="R9" s="1">
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
-      <c r="S9" s="1">
+      <c r="T9" s="1">
         <f t="shared" si="9"/>
         <v>8</v>
       </c>
-      <c r="U9" s="1">
+      <c r="V9" s="1">
         <f t="shared" si="10"/>
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+    <row r="10" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D10" s="1">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="G10" s="1">
+      <c r="H10" s="1">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="I10" s="1">
+      <c r="J10" s="1">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K10" s="1">
+      <c r="K10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L10" s="1">
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="M10" s="1">
+      <c r="N10" s="1">
         <f t="shared" si="6"/>
         <v>9</v>
       </c>
-      <c r="O10" s="1">
+      <c r="P10" s="1">
         <f t="shared" si="7"/>
         <v>9</v>
       </c>
-      <c r="Q10" s="1">
+      <c r="R10" s="1">
         <f t="shared" si="8"/>
         <v>9</v>
       </c>
-      <c r="S10" s="1">
+      <c r="T10" s="1">
         <f t="shared" si="9"/>
         <v>9</v>
       </c>
-      <c r="U10" s="1">
+      <c r="V10" s="1">
         <f t="shared" si="10"/>
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+    <row r="11" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D11" s="1">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F11" s="1">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="G11" s="1">
+      <c r="H11" s="1">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="I11" s="1">
+      <c r="J11" s="1">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="K11" s="1">
+      <c r="L11" s="1">
         <f t="shared" si="5"/>
         <v>10</v>
       </c>
-      <c r="M11" s="1">
+      <c r="N11" s="1">
         <f t="shared" si="6"/>
         <v>10</v>
       </c>
-      <c r="O11" s="1">
+      <c r="P11" s="1">
         <f t="shared" si="7"/>
         <v>10</v>
       </c>
-      <c r="Q11" s="1">
+      <c r="R11" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
-      <c r="S11" s="1">
+      <c r="T11" s="1">
         <f t="shared" si="9"/>
         <v>10</v>
       </c>
-      <c r="U11" s="1">
+      <c r="V11" s="1">
         <f t="shared" si="10"/>
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+    <row r="12" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D12" s="1">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="E12" s="1">
+      <c r="F12" s="1">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="G12" s="1">
+      <c r="H12" s="1">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="I12" s="1">
+      <c r="J12" s="1">
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
-      <c r="K12" s="1">
+      <c r="L12" s="1">
         <f t="shared" si="5"/>
         <v>11</v>
       </c>
-      <c r="M12" s="1">
+      <c r="N12" s="1">
         <f t="shared" si="6"/>
         <v>11</v>
       </c>
-      <c r="O12" s="1">
+      <c r="P12" s="1">
         <f t="shared" si="7"/>
         <v>11</v>
       </c>
-      <c r="Q12" s="1">
+      <c r="R12" s="1">
         <f t="shared" si="8"/>
         <v>11</v>
       </c>
-      <c r="S12" s="1">
+      <c r="T12" s="1">
         <f t="shared" si="9"/>
         <v>11</v>
       </c>
-      <c r="U12" s="1">
+      <c r="V12" s="1">
         <f t="shared" si="10"/>
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+    <row r="13" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C13" s="1">
+      <c r="D13" s="1">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="1">
+      <c r="E13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="1">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="G13" s="1">
+      <c r="H13" s="1">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="I13" s="1">
+      <c r="J13" s="1">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="K13" s="1">
+      <c r="L13" s="1">
         <f t="shared" si="5"/>
         <v>12</v>
       </c>
-      <c r="M13" s="1">
+      <c r="N13" s="1">
         <f t="shared" si="6"/>
         <v>12</v>
       </c>
-      <c r="O13" s="1">
+      <c r="P13" s="1">
         <f t="shared" si="7"/>
         <v>12</v>
       </c>
-      <c r="Q13" s="1">
+      <c r="R13" s="1">
         <f t="shared" si="8"/>
         <v>12</v>
       </c>
-      <c r="S13" s="1">
+      <c r="T13" s="1">
         <f t="shared" si="9"/>
         <v>12</v>
       </c>
-      <c r="U13" s="1">
+      <c r="V13" s="1">
         <f t="shared" si="10"/>
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+    <row r="14" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C14" s="1">
+      <c r="D14" s="1">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="E14" s="1">
+      <c r="F14" s="1">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="G14" s="1">
+      <c r="H14" s="1">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="I14" s="1">
+      <c r="J14" s="1">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
-      <c r="K14" s="1">
+      <c r="L14" s="1">
         <f t="shared" si="5"/>
         <v>13</v>
       </c>
-      <c r="M14" s="1">
+      <c r="N14" s="1">
         <f t="shared" si="6"/>
         <v>13</v>
       </c>
-      <c r="O14" s="1">
+      <c r="P14" s="1">
         <f t="shared" si="7"/>
         <v>13</v>
       </c>
-      <c r="Q14" s="1">
+      <c r="R14" s="1">
         <f t="shared" si="8"/>
         <v>13</v>
       </c>
-      <c r="S14" s="1">
+      <c r="T14" s="1">
         <f t="shared" si="9"/>
         <v>13</v>
       </c>
-      <c r="U14" s="1">
+      <c r="V14" s="1">
         <f t="shared" si="10"/>
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+    <row r="15" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C15" s="1">
+      <c r="D15" s="1">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="E15" s="1">
+      <c r="F15" s="1">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="G15" s="1">
+      <c r="H15" s="1">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="I15" s="1">
+      <c r="J15" s="1">
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="K15" s="1">
+      <c r="L15" s="1">
         <f t="shared" si="5"/>
         <v>14</v>
       </c>
-      <c r="M15" s="1">
+      <c r="N15" s="1">
         <f t="shared" si="6"/>
         <v>14</v>
       </c>
-      <c r="O15" s="1">
+      <c r="P15" s="1">
         <f t="shared" si="7"/>
         <v>14</v>
       </c>
-      <c r="Q15" s="1">
+      <c r="R15" s="1">
         <f t="shared" si="8"/>
         <v>14</v>
       </c>
-      <c r="S15" s="1">
+      <c r="T15" s="1">
         <f t="shared" si="9"/>
         <v>14</v>
       </c>
-      <c r="U15" s="1">
+      <c r="V15" s="1">
         <f t="shared" si="10"/>
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+    <row r="16" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C16" s="1">
+      <c r="D16" s="1">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="E16" s="1">
+      <c r="F16" s="1">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="G16" s="1">
+      <c r="H16" s="1">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="I16" s="1">
+      <c r="J16" s="1">
         <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="K16" s="1">
+      <c r="L16" s="1">
         <f t="shared" si="5"/>
         <v>15</v>
       </c>
-      <c r="M16" s="1">
+      <c r="N16" s="1">
         <f t="shared" si="6"/>
         <v>15</v>
       </c>
-      <c r="O16" s="1">
+      <c r="P16" s="1">
         <f t="shared" si="7"/>
         <v>15</v>
       </c>
-      <c r="Q16" s="1">
+      <c r="R16" s="1">
         <f t="shared" si="8"/>
         <v>15</v>
       </c>
-      <c r="S16" s="1">
+      <c r="T16" s="1">
         <f t="shared" si="9"/>
         <v>15</v>
       </c>
-      <c r="U16" s="1">
+      <c r="V16" s="1">
         <f t="shared" si="10"/>
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C17" s="1">
+      <c r="D17" s="1">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="E17" s="1">
+      <c r="F17" s="1">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="G17" s="1">
+      <c r="H17" s="1">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="I17" s="1">
+      <c r="J17" s="1">
         <f t="shared" si="4"/>
         <v>16</v>
       </c>
-      <c r="K17" s="1">
+      <c r="L17" s="1">
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
-      <c r="M17" s="1">
+      <c r="N17" s="1">
         <f t="shared" si="6"/>
         <v>16</v>
       </c>
-      <c r="O17" s="1">
+      <c r="P17" s="1">
         <f t="shared" si="7"/>
         <v>16</v>
       </c>
-      <c r="Q17" s="1">
+      <c r="R17" s="1">
         <f t="shared" si="8"/>
         <v>16</v>
       </c>
-      <c r="S17" s="1">
+      <c r="T17" s="1">
         <f t="shared" si="9"/>
         <v>16</v>
       </c>
-      <c r="U17" s="1">
+      <c r="V17" s="1">
         <f t="shared" si="10"/>
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C18" s="1">
+      <c r="D18" s="1">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="E18" s="1">
+      <c r="F18" s="1">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="G18" s="1">
+      <c r="H18" s="1">
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
-      <c r="I18" s="1">
+      <c r="J18" s="1">
         <f t="shared" si="4"/>
         <v>17</v>
       </c>
-      <c r="K18" s="1">
+      <c r="L18" s="1">
         <f t="shared" si="5"/>
         <v>17</v>
       </c>
-      <c r="M18" s="1">
+      <c r="N18" s="1">
         <f t="shared" si="6"/>
         <v>17</v>
       </c>
-      <c r="O18" s="1">
+      <c r="P18" s="1">
         <f t="shared" si="7"/>
         <v>17</v>
       </c>
-      <c r="Q18" s="1">
+      <c r="R18" s="1">
         <f t="shared" si="8"/>
         <v>17</v>
       </c>
-      <c r="S18" s="1">
+      <c r="T18" s="1">
         <f t="shared" si="9"/>
         <v>17</v>
       </c>
-      <c r="U18" s="1">
-        <f>U17+1</f>
+      <c r="V18" s="1">
+        <f>V17+1</f>
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="1">
+      <c r="C19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="E19" s="1">
+      <c r="F19" s="1">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="G19" s="1">
+      <c r="H19" s="1">
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
-      <c r="I19" s="1">
+      <c r="J19" s="1">
         <f t="shared" si="4"/>
         <v>18</v>
       </c>
-      <c r="K19" s="1">
+      <c r="L19" s="1">
         <f t="shared" si="5"/>
         <v>18</v>
       </c>
-      <c r="M19" s="1">
+      <c r="N19" s="1">
         <f t="shared" si="6"/>
         <v>18</v>
       </c>
-      <c r="O19" s="1">
+      <c r="P19" s="1">
         <f t="shared" si="7"/>
         <v>18</v>
       </c>
-      <c r="Q19" s="1">
+      <c r="R19" s="1">
         <f t="shared" si="8"/>
         <v>18</v>
       </c>
-      <c r="S19" s="1">
+      <c r="T19" s="1">
         <f t="shared" si="9"/>
         <v>18</v>
       </c>
-      <c r="U19" s="1">
+      <c r="V19" s="1">
         <f t="shared" si="10"/>
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+    <row r="20" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B20" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C20" s="1">
+      <c r="D20" s="1">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="E20" s="1">
+      <c r="F20" s="1">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="G20" s="1">
+      <c r="H20" s="1">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="I20" s="1">
+      <c r="J20" s="1">
         <f t="shared" si="4"/>
         <v>19</v>
       </c>
-      <c r="K20" s="1">
+      <c r="L20" s="1">
         <f t="shared" si="5"/>
         <v>19</v>
       </c>
-      <c r="M20" s="1">
+      <c r="N20" s="1">
         <f t="shared" si="6"/>
         <v>19</v>
       </c>
-      <c r="O20" s="1">
+      <c r="P20" s="1">
         <f t="shared" si="7"/>
         <v>19</v>
       </c>
-      <c r="Q20" s="1">
+      <c r="R20" s="1">
         <f t="shared" si="8"/>
         <v>19</v>
       </c>
-      <c r="S20" s="1">
+      <c r="T20" s="1">
         <f t="shared" si="9"/>
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+    <row r="21" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C21" s="1">
+      <c r="D21" s="1">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="E21" s="1">
+      <c r="F21" s="1">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="G21" s="1">
+      <c r="H21" s="1">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="I21" s="1">
+      <c r="J21" s="1">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
-      <c r="M21" s="1">
+      <c r="N21" s="1">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
-      <c r="O21" s="1">
+      <c r="P21" s="1">
         <f t="shared" si="7"/>
         <v>20</v>
       </c>
-      <c r="Q21" s="1">
+      <c r="R21" s="1">
         <f t="shared" si="8"/>
         <v>20</v>
       </c>
-      <c r="S21" s="1">
+      <c r="T21" s="1">
         <f t="shared" si="9"/>
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C22" s="1">
+    <row r="22" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="D22" s="1">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="E22" s="1">
+      <c r="F22" s="1">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="G22" s="1">
+      <c r="H22" s="1">
         <f t="shared" si="3"/>
         <v>21</v>
       </c>
-      <c r="I22" s="1">
+      <c r="J22" s="1">
         <f t="shared" si="4"/>
         <v>21</v>
       </c>
-      <c r="M22" s="1">
+      <c r="N22" s="1">
         <f t="shared" si="6"/>
         <v>21</v>
       </c>
-      <c r="O22" s="1">
+      <c r="P22" s="1">
         <f t="shared" si="7"/>
         <v>21</v>
       </c>
-      <c r="Q22" s="1">
+      <c r="R22" s="1">
         <f t="shared" si="8"/>
         <v>21</v>
       </c>
-      <c r="S22" s="1">
+      <c r="T22" s="1">
         <f t="shared" si="9"/>
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C23" s="1">
+    <row r="23" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="D23" s="1">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="E23" s="1">
+      <c r="F23" s="1">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="G23" s="1">
+      <c r="H23" s="1">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
-      <c r="I23" s="1">
+      <c r="J23" s="1">
         <f t="shared" si="4"/>
         <v>22</v>
       </c>
-      <c r="M23" s="1">
+      <c r="N23" s="1">
         <f t="shared" si="6"/>
         <v>22</v>
       </c>
-      <c r="O23" s="1">
+      <c r="P23" s="1">
         <f t="shared" si="7"/>
         <v>22</v>
       </c>
-      <c r="Q23" s="1">
+      <c r="R23" s="1">
         <f t="shared" si="8"/>
         <v>22</v>
       </c>
-      <c r="S23" s="1">
+      <c r="T23" s="1">
         <f t="shared" si="9"/>
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C24" s="1">
+    <row r="24" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="D24" s="1">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="E24" s="1">
+      <c r="F24" s="1">
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="G24" s="1">
+      <c r="H24" s="1">
         <f t="shared" si="3"/>
         <v>23</v>
       </c>
-      <c r="I24" s="1">
+      <c r="J24" s="1">
         <f t="shared" si="4"/>
         <v>23</v>
       </c>
-      <c r="M24" s="1">
+      <c r="N24" s="1">
         <f t="shared" si="6"/>
         <v>23</v>
       </c>
-      <c r="O24" s="1">
+      <c r="P24" s="1">
         <f t="shared" si="7"/>
         <v>23</v>
       </c>
-      <c r="Q24" s="1">
+      <c r="R24" s="1">
         <f t="shared" si="8"/>
         <v>23</v>
       </c>
-      <c r="S24" s="1">
+      <c r="T24" s="1">
         <f t="shared" si="9"/>
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C25" s="1">
+    <row r="25" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="D25" s="1">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="E25" s="1">
+      <c r="F25" s="1">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="G25" s="1">
+      <c r="H25" s="1">
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="I25" s="1">
+      <c r="J25" s="1">
         <f t="shared" si="4"/>
         <v>24</v>
       </c>
-      <c r="M25" s="1">
+      <c r="N25" s="1">
         <f t="shared" si="6"/>
         <v>24</v>
       </c>
-      <c r="O25" s="1">
+      <c r="P25" s="1">
         <f t="shared" si="7"/>
         <v>24</v>
       </c>
-      <c r="Q25" s="1">
+      <c r="R25" s="1">
         <f t="shared" si="8"/>
         <v>24</v>
       </c>
-      <c r="S25" s="1">
+      <c r="T25" s="1">
         <f t="shared" si="9"/>
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C26" s="1">
+    <row r="26" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="D26" s="1">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="E26" s="1">
+      <c r="F26" s="1">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="G26" s="1">
+      <c r="H26" s="1">
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="I26" s="1">
+      <c r="J26" s="1">
         <f t="shared" si="4"/>
         <v>25</v>
       </c>
-      <c r="M26" s="1">
+      <c r="N26" s="1">
         <f t="shared" si="6"/>
         <v>25</v>
       </c>
-      <c r="O26" s="1">
+      <c r="P26" s="1">
         <f t="shared" si="7"/>
         <v>25</v>
       </c>
-      <c r="Q26" s="1">
+      <c r="R26" s="1">
         <f t="shared" si="8"/>
         <v>25</v>
       </c>
-      <c r="S26" s="1">
+      <c r="T26" s="1">
         <f t="shared" si="9"/>
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C27" s="1">
+    <row r="27" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="D27" s="1">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="G27" s="1">
+      <c r="H27" s="1">
         <f t="shared" si="3"/>
         <v>26</v>
       </c>
-      <c r="I27" s="1">
+      <c r="J27" s="1">
         <f t="shared" si="4"/>
         <v>26</v>
       </c>
-      <c r="M27" s="1">
+      <c r="N27" s="1">
         <f t="shared" si="6"/>
         <v>26</v>
       </c>
-      <c r="O27" s="1">
+      <c r="P27" s="1">
         <f t="shared" si="7"/>
         <v>26</v>
       </c>
-      <c r="Q27" s="1">
+      <c r="R27" s="1">
         <f t="shared" si="8"/>
         <v>26</v>
       </c>
-      <c r="S27" s="1">
+      <c r="T27" s="1">
         <f t="shared" si="9"/>
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C28" s="1">
+    <row r="28" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="D28" s="1">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="I28" s="1">
+      <c r="J28" s="1">
         <f t="shared" si="4"/>
         <v>27</v>
       </c>
-      <c r="O28" s="1">
+      <c r="P28" s="1">
         <f t="shared" si="7"/>
         <v>27</v>
       </c>
-      <c r="Q28" s="1">
+      <c r="R28" s="1">
         <f t="shared" si="8"/>
         <v>27</v>
       </c>
-      <c r="S28" s="1">
+      <c r="T28" s="1">
         <f t="shared" si="9"/>
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C29" s="1">
+    <row r="29" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="D29" s="1">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="I29" s="1">
+      <c r="J29" s="1">
         <f t="shared" si="4"/>
         <v>28</v>
       </c>
-      <c r="O29" s="1">
+      <c r="P29" s="1">
         <f t="shared" si="7"/>
         <v>28</v>
       </c>
-      <c r="Q29" s="1">
+      <c r="R29" s="1">
         <f t="shared" si="8"/>
         <v>28</v>
       </c>
-      <c r="S29" s="1">
+      <c r="T29" s="1">
         <f t="shared" si="9"/>
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C30" s="1">
+    <row r="30" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="D30" s="1">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="I30" s="1">
+      <c r="J30" s="1">
         <f t="shared" si="4"/>
         <v>29</v>
       </c>
-      <c r="O30" s="1">
+      <c r="P30" s="1">
         <f t="shared" si="7"/>
         <v>29</v>
       </c>
-      <c r="Q30" s="1">
+      <c r="R30" s="1">
         <f t="shared" si="8"/>
         <v>29</v>
       </c>
-      <c r="S30" s="1">
+      <c r="T30" s="1">
         <f t="shared" si="9"/>
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C31" s="1">
-        <f>C30+1</f>
+    <row r="31" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="D31" s="1">
+        <f>D30+1</f>
         <v>30</v>
       </c>
-      <c r="O31" s="1">
+      <c r="P31" s="1">
         <f t="shared" si="7"/>
         <v>30</v>
       </c>
-      <c r="Q31" s="1">
+      <c r="R31" s="1">
         <f t="shared" si="8"/>
         <v>30</v>
       </c>
-      <c r="S31" s="1">
+      <c r="T31" s="1">
         <f t="shared" si="9"/>
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="O32" s="1">
+    <row r="32" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="P32" s="1">
         <f t="shared" si="7"/>
         <v>31</v>
       </c>
-      <c r="Q32" s="1">
+      <c r="R32" s="1">
         <f t="shared" si="8"/>
         <v>31</v>
       </c>
-      <c r="S32" s="1">
+      <c r="T32" s="1">
         <f t="shared" si="9"/>
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S33" s="1">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="T33" s="1">
         <f t="shared" si="9"/>
         <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="C35" s="1" t="str">
+        <f>B$1</f>
+        <v>Chapter 1</v>
+      </c>
+      <c r="E35" s="1" t="str">
+        <f t="shared" ref="D35:W35" si="11">D$1</f>
+        <v>Chapter 2</v>
+      </c>
+      <c r="G35" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>Chapter 3</v>
+      </c>
+      <c r="I35" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>Chapter 4</v>
+      </c>
+      <c r="K35" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>Chapter 5</v>
+      </c>
+      <c r="M35" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>Chapter 6</v>
+      </c>
+      <c r="O35" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>Chapter 7</v>
+      </c>
+      <c r="Q35" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>Chapter 8</v>
+      </c>
+      <c r="S35" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>Chapter 9</v>
+      </c>
+      <c r="U35" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>Chapter 10</v>
+      </c>
+      <c r="W35" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>Chapter 11</v>
+      </c>
+      <c r="Y35" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="1">
+        <f>COUNTIF(C$2:C$33,"In Progress")</f>
+        <v>0</v>
+      </c>
+      <c r="E36" s="1">
+        <f t="shared" ref="E36:W36" si="12">COUNTIF(E$2:E$33,"In Progress")</f>
+        <v>0</v>
+      </c>
+      <c r="G36" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="I36" s="1">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="K36" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="M36" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O36" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="Q36" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="S36" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="U36" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="W36" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="X36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y36" s="1">
+        <f>SUM(C36:W36)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="1">
+        <f>COUNTIF(C$2:C$33,"Completed")</f>
+        <v>6</v>
+      </c>
+      <c r="E37" s="1">
+        <f t="shared" ref="E37:W37" si="13">COUNTIF(E$2:E$33,"Completed")</f>
+        <v>2</v>
+      </c>
+      <c r="G37" s="1">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="I37" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="K37" s="1">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="M37" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="O37" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="Q37" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="S37" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="U37" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="W37" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="X37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y37" s="1">
+        <f t="shared" ref="Y37:Y38" si="14">SUM(C37:W37)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="1">
+        <f>COUNT(B$2:B$33)</f>
+        <v>20</v>
+      </c>
+      <c r="E38" s="1">
+        <f t="shared" ref="E38:W38" si="15">COUNT(D$2:D$33)</f>
+        <v>30</v>
+      </c>
+      <c r="G38" s="1">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="I38" s="1">
+        <f t="shared" si="15"/>
+        <v>26</v>
+      </c>
+      <c r="K38" s="1">
+        <f t="shared" si="15"/>
+        <v>29</v>
+      </c>
+      <c r="M38" s="1">
+        <f t="shared" si="15"/>
+        <v>19</v>
+      </c>
+      <c r="O38" s="1">
+        <f t="shared" si="15"/>
+        <v>26</v>
+      </c>
+      <c r="Q38" s="1">
+        <f t="shared" si="15"/>
+        <v>31</v>
+      </c>
+      <c r="S38" s="1">
+        <f t="shared" si="15"/>
+        <v>31</v>
+      </c>
+      <c r="U38" s="1">
+        <f t="shared" si="15"/>
+        <v>32</v>
+      </c>
+      <c r="W38" s="1">
+        <f t="shared" si="15"/>
+        <v>18</v>
+      </c>
+      <c r="X38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y38" s="1">
+        <f t="shared" si="14"/>
+        <v>287</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="3">
+        <f>C$37/C$38</f>
+        <v>0.3</v>
+      </c>
+      <c r="E39" s="3">
+        <f>E$37/E$38</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="G39" s="3">
+        <f>G$37/G$38</f>
+        <v>0.04</v>
+      </c>
+      <c r="I39" s="3">
+        <f>I$37/I$38</f>
+        <v>0</v>
+      </c>
+      <c r="K39" s="3">
+        <f>K$37/K$38</f>
+        <v>3.4482758620689655E-2</v>
+      </c>
+      <c r="M39" s="3">
+        <f>M$37/M$38</f>
+        <v>0</v>
+      </c>
+      <c r="O39" s="3">
+        <f>O$37/O$38</f>
+        <v>0</v>
+      </c>
+      <c r="Q39" s="3">
+        <f>Q$37/Q$38</f>
+        <v>0</v>
+      </c>
+      <c r="S39" s="3">
+        <f>S$37/S$38</f>
+        <v>0</v>
+      </c>
+      <c r="U39" s="3">
+        <f>U$37/U$38</f>
+        <v>0</v>
+      </c>
+      <c r="W39" s="3">
+        <f>W$37/W$38</f>
+        <v>0</v>
+      </c>
+      <c r="X39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y39" s="3">
+        <f>Y37/Y38</f>
+        <v>3.484320557491289E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{3E9AD461-33FE-4C12-BC5D-6843F8759F43}">
+            <xm:f>NOT(ISERROR(SEARCH(Sheet2!$A$3,C2)))</xm:f>
+            <xm:f>Sheet2!$A$3</xm:f>
+            <x14:dxf>
+              <font>
+                <strike val="0"/>
+                <color theme="0"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFEEC00"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
           <x14:cfRule type="containsText" priority="2" operator="containsText" id="{83F44093-A430-4148-9498-2DA9893DB6C7}">
-            <xm:f>NOT(ISERROR(SEARCH(Sheet2!$A$4,B2)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH(Sheet2!$A$4,C2)))</xm:f>
             <xm:f>Sheet2!$A$4</xm:f>
             <x14:dxf>
               <font>
@@ -1845,22 +2148,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{3E9AD461-33FE-4C12-BC5D-6843F8759F43}">
-            <xm:f>NOT(ISERROR(SEARCH(Sheet2!$A$3,B2)))</xm:f>
-            <xm:f>Sheet2!$A$3</xm:f>
-            <x14:dxf>
-              <font>
-                <strike val="0"/>
-                <color theme="0"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFEEC00"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>D2:D31 F2:F26 H2:H27 B2:B21 J2:J30 L2:L20 N2:N27 P2:P32 R2:R32 T2:T33 V2:V19</xm:sqref>
+          <xm:sqref>E2:E31 G2:G26 I2:I27 C2:C21 K2:K30 M2:M20 O2:O27 Q2:Q32 S2:S32 U2:U34 W2:W19 U36</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1870,7 +2158,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D31 F2:F26 H2:H27 B2:B21 J2:J30 L2:L20 N2:N27 P2:P32 R2:R32 T2:T33 V2:V19</xm:sqref>
+          <xm:sqref>E2:E31 G2:G26 I2:I27 C2:C21 K2:K30 M2:M20 O2:O27 Q2:Q32 S2:S32 W2:W19 U2:U34 U36</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Finished Chapter 4 Exercise 14
</commit_message>
<xml_diff>
--- a/Principles of Mathematical Analysis - Progress.xlsx
+++ b/Principles of Mathematical Analysis - Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TeX\Books\Rudin, Walter\Principles of Mathematical Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3828EDF8-9991-4FCA-B74E-D61B22347757}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77EEB260-D55C-4B8A-9BA9-7B9183E001B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4ECAD2DA-16DF-447C-94EF-7D164C966ED4}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
   <si>
     <t>Status</t>
   </si>
@@ -90,12 +90,15 @@
   <si>
     <t>Total</t>
   </si>
+  <si>
+    <t>Awaiting Write-up</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,13 +113,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -132,24 +149,151 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEEC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFF30D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEEC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEEC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -256,6 +400,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCC0000"/>
+      <color rgb="FFFFF30D"/>
       <color rgb="FFFEEC00"/>
       <color rgb="FFFFFF66"/>
     </mruColors>
@@ -568,90 +714,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EB77106-B98B-4FF2-B67C-6A4D8C99C21E}">
-  <dimension ref="A1:Y39"/>
+  <dimension ref="A1:AE59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="Y39" activeCellId="11" sqref="C39 E39 G39 I39 K39 M39 O39 Q39 S39 U39 W39 Y39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="3.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="3.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="3.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" style="1" customWidth="1"/>
     <col min="10" max="10" width="3.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" style="1" customWidth="1"/>
     <col min="12" max="12" width="3.42578125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="18.28515625" style="1" customWidth="1"/>
     <col min="14" max="14" width="3.42578125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="18.28515625" style="1" customWidth="1"/>
     <col min="16" max="16" width="3.42578125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="13.7109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="18.28515625" style="1" customWidth="1"/>
     <col min="18" max="18" width="3.42578125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.7109375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="18.28515625" style="1" customWidth="1"/>
     <col min="20" max="20" width="3.42578125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="13.7109375" style="1" customWidth="1"/>
+    <col min="21" max="21" width="18.28515625" style="1" customWidth="1"/>
     <col min="22" max="22" width="3.42578125" style="1" customWidth="1"/>
-    <col min="23" max="23" width="13.7109375" style="1" customWidth="1"/>
+    <col min="23" max="23" width="18.28515625" style="1" customWidth="1"/>
     <col min="24" max="24" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="5"/>
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="G1" s="5"/>
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2" t="s">
+      <c r="I1" s="5"/>
+      <c r="J1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2" t="s">
+      <c r="K1" s="5"/>
+      <c r="L1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2" t="s">
+      <c r="M1" s="5"/>
+      <c r="N1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2" t="s">
+      <c r="O1" s="5"/>
+      <c r="P1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2" t="s">
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2" t="s">
+      <c r="S1" s="5"/>
+      <c r="T1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2" t="s">
+      <c r="U1" s="5"/>
+      <c r="V1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="W1" s="2"/>
+      <c r="W1" s="5"/>
       <c r="X1" s="4"/>
       <c r="Y1" s="4"/>
-    </row>
-    <row r="2" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="3"/>
+      <c r="AE1" s="3"/>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
       <c r="B2" s="1">
         <v>1</v>
       </c>
@@ -697,8 +851,17 @@
       <c r="V2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+      <c r="AE2" s="3"/>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
       <c r="B3" s="1">
         <f>B2+1</f>
         <v>2</v>
@@ -746,8 +909,17 @@
         <f>V2+1</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AE3" s="3"/>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
       <c r="B4" s="1">
         <f t="shared" ref="B4:B21" si="0">B3+1</f>
         <v>3</v>
@@ -795,8 +967,17 @@
         <f t="shared" ref="V4:V19" si="10">V3+1</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="3"/>
+      <c r="AE4" s="3"/>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
       <c r="B5" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -844,8 +1025,17 @@
         <f t="shared" si="10"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3"/>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
       <c r="B6" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -893,8 +1083,17 @@
         <f t="shared" si="10"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
       <c r="B7" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -939,8 +1138,17 @@
         <f t="shared" si="10"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
       <c r="B8" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -985,12 +1193,24 @@
         <f t="shared" si="10"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
+      <c r="AE8" s="3"/>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
       <c r="B9" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="D9" s="1">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -1031,8 +1251,17 @@
         <f t="shared" si="10"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="3"/>
+      <c r="AE9" s="3"/>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
       <c r="B10" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1080,8 +1309,17 @@
         <f t="shared" si="10"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="3"/>
+      <c r="AC10" s="3"/>
+      <c r="AD10" s="3"/>
+      <c r="AE10" s="3"/>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
       <c r="B11" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1126,8 +1364,17 @@
         <f t="shared" si="10"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="3"/>
+      <c r="AB11" s="3"/>
+      <c r="AC11" s="3"/>
+      <c r="AD11" s="3"/>
+      <c r="AE11" s="3"/>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
       <c r="B12" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1172,8 +1419,17 @@
         <f t="shared" si="10"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3"/>
+      <c r="AA12" s="3"/>
+      <c r="AB12" s="3"/>
+      <c r="AC12" s="3"/>
+      <c r="AD12" s="3"/>
+      <c r="AE12" s="3"/>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
       <c r="B13" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1221,12 +1477,24 @@
         <f t="shared" si="10"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="X13" s="3"/>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="3"/>
+      <c r="AA13" s="3"/>
+      <c r="AB13" s="3"/>
+      <c r="AC13" s="3"/>
+      <c r="AD13" s="3"/>
+      <c r="AE13" s="3"/>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
       <c r="B14" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
+      <c r="C14" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="D14" s="1">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -1267,8 +1535,17 @@
         <f t="shared" si="10"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="X14" s="3"/>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="3"/>
+      <c r="AA14" s="3"/>
+      <c r="AB14" s="3"/>
+      <c r="AC14" s="3"/>
+      <c r="AD14" s="3"/>
+      <c r="AE14" s="3"/>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
       <c r="B15" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1313,8 +1590,17 @@
         <f t="shared" si="10"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="X15" s="3"/>
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="3"/>
+      <c r="AA15" s="3"/>
+      <c r="AB15" s="3"/>
+      <c r="AC15" s="3"/>
+      <c r="AD15" s="3"/>
+      <c r="AE15" s="3"/>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
       <c r="B16" s="1">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1359,8 +1645,17 @@
         <f t="shared" si="10"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="X16" s="3"/>
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="3"/>
+      <c r="AA16" s="3"/>
+      <c r="AB16" s="3"/>
+      <c r="AC16" s="3"/>
+      <c r="AD16" s="3"/>
+      <c r="AE16" s="3"/>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
       <c r="B17" s="1">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1405,12 +1700,24 @@
         <f t="shared" si="10"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="X17" s="3"/>
+      <c r="Y17" s="3"/>
+      <c r="Z17" s="3"/>
+      <c r="AA17" s="3"/>
+      <c r="AB17" s="3"/>
+      <c r="AC17" s="3"/>
+      <c r="AD17" s="3"/>
+      <c r="AE17" s="3"/>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
       <c r="B18" s="1">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
+      <c r="C18" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="D18" s="1">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -1451,8 +1758,17 @@
         <f>V17+1</f>
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="X18" s="3"/>
+      <c r="Y18" s="3"/>
+      <c r="Z18" s="3"/>
+      <c r="AA18" s="3"/>
+      <c r="AB18" s="3"/>
+      <c r="AC18" s="3"/>
+      <c r="AD18" s="3"/>
+      <c r="AE18" s="3"/>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
       <c r="B19" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1500,8 +1816,17 @@
         <f t="shared" si="10"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="X19" s="3"/>
+      <c r="Y19" s="3"/>
+      <c r="Z19" s="3"/>
+      <c r="AA19" s="3"/>
+      <c r="AB19" s="3"/>
+      <c r="AC19" s="3"/>
+      <c r="AD19" s="3"/>
+      <c r="AE19" s="3"/>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
       <c r="B20" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1542,8 +1867,19 @@
         <f t="shared" si="9"/>
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="V20" s="3"/>
+      <c r="W20" s="3"/>
+      <c r="X20" s="3"/>
+      <c r="Y20" s="3"/>
+      <c r="Z20" s="3"/>
+      <c r="AA20" s="3"/>
+      <c r="AB20" s="3"/>
+      <c r="AC20" s="3"/>
+      <c r="AD20" s="3"/>
+      <c r="AE20" s="3"/>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
       <c r="B21" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1564,6 +1900,8 @@
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
       <c r="N21" s="1">
         <f t="shared" si="6"/>
         <v>20</v>
@@ -1580,8 +1918,21 @@
         <f t="shared" si="9"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="V21" s="3"/>
+      <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
+      <c r="Y21" s="3"/>
+      <c r="Z21" s="3"/>
+      <c r="AA21" s="3"/>
+      <c r="AB21" s="3"/>
+      <c r="AC21" s="3"/>
+      <c r="AD21" s="3"/>
+      <c r="AE21" s="3"/>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
       <c r="D22" s="1">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -1598,6 +1949,8 @@
         <f t="shared" si="4"/>
         <v>21</v>
       </c>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
       <c r="N22" s="1">
         <f t="shared" si="6"/>
         <v>21</v>
@@ -1614,8 +1967,21 @@
         <f t="shared" si="9"/>
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="V22" s="3"/>
+      <c r="W22" s="3"/>
+      <c r="X22" s="3"/>
+      <c r="Y22" s="3"/>
+      <c r="Z22" s="3"/>
+      <c r="AA22" s="3"/>
+      <c r="AB22" s="3"/>
+      <c r="AC22" s="3"/>
+      <c r="AD22" s="3"/>
+      <c r="AE22" s="3"/>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
       <c r="D23" s="1">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -1632,6 +1998,8 @@
         <f t="shared" si="4"/>
         <v>22</v>
       </c>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
       <c r="N23" s="1">
         <f t="shared" si="6"/>
         <v>22</v>
@@ -1648,8 +2016,21 @@
         <f t="shared" si="9"/>
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="V23" s="3"/>
+      <c r="W23" s="3"/>
+      <c r="X23" s="3"/>
+      <c r="Y23" s="3"/>
+      <c r="Z23" s="3"/>
+      <c r="AA23" s="3"/>
+      <c r="AB23" s="3"/>
+      <c r="AC23" s="3"/>
+      <c r="AD23" s="3"/>
+      <c r="AE23" s="3"/>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
       <c r="D24" s="1">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -1666,6 +2047,8 @@
         <f t="shared" si="4"/>
         <v>23</v>
       </c>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
       <c r="N24" s="1">
         <f t="shared" si="6"/>
         <v>23</v>
@@ -1682,8 +2065,21 @@
         <f t="shared" si="9"/>
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="V24" s="3"/>
+      <c r="W24" s="3"/>
+      <c r="X24" s="3"/>
+      <c r="Y24" s="3"/>
+      <c r="Z24" s="3"/>
+      <c r="AA24" s="3"/>
+      <c r="AB24" s="3"/>
+      <c r="AC24" s="3"/>
+      <c r="AD24" s="3"/>
+      <c r="AE24" s="3"/>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
       <c r="D25" s="1">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -1700,6 +2096,8 @@
         <f t="shared" si="4"/>
         <v>24</v>
       </c>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
       <c r="N25" s="1">
         <f t="shared" si="6"/>
         <v>24</v>
@@ -1716,8 +2114,21 @@
         <f t="shared" si="9"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="V25" s="3"/>
+      <c r="W25" s="3"/>
+      <c r="X25" s="3"/>
+      <c r="Y25" s="3"/>
+      <c r="Z25" s="3"/>
+      <c r="AA25" s="3"/>
+      <c r="AB25" s="3"/>
+      <c r="AC25" s="3"/>
+      <c r="AD25" s="3"/>
+      <c r="AE25" s="3"/>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
       <c r="D26" s="1">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -1734,6 +2145,8 @@
         <f t="shared" si="4"/>
         <v>25</v>
       </c>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
       <c r="N26" s="1">
         <f t="shared" si="6"/>
         <v>25</v>
@@ -1750,12 +2163,27 @@
         <f t="shared" si="9"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="V26" s="3"/>
+      <c r="W26" s="3"/>
+      <c r="X26" s="3"/>
+      <c r="Y26" s="3"/>
+      <c r="Z26" s="3"/>
+      <c r="AA26" s="3"/>
+      <c r="AB26" s="3"/>
+      <c r="AC26" s="3"/>
+      <c r="AD26" s="3"/>
+      <c r="AE26" s="3"/>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
       <c r="D27" s="1">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
       <c r="H27" s="1">
         <f t="shared" si="3"/>
         <v>26</v>
@@ -1764,6 +2192,8 @@
         <f t="shared" si="4"/>
         <v>26</v>
       </c>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
       <c r="N27" s="1">
         <f t="shared" si="6"/>
         <v>26</v>
@@ -1780,16 +2210,37 @@
         <f t="shared" si="9"/>
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="V27" s="3"/>
+      <c r="W27" s="3"/>
+      <c r="X27" s="3"/>
+      <c r="Y27" s="3"/>
+      <c r="Z27" s="3"/>
+      <c r="AA27" s="3"/>
+      <c r="AB27" s="3"/>
+      <c r="AC27" s="3"/>
+      <c r="AD27" s="3"/>
+      <c r="AE27" s="3"/>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
       <c r="D28" s="1">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
       <c r="J28" s="1">
         <f t="shared" si="4"/>
         <v>27</v>
       </c>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
       <c r="P28" s="1">
         <f t="shared" si="7"/>
         <v>27</v>
@@ -1802,16 +2253,37 @@
         <f t="shared" si="9"/>
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="V28" s="3"/>
+      <c r="W28" s="3"/>
+      <c r="X28" s="3"/>
+      <c r="Y28" s="3"/>
+      <c r="Z28" s="3"/>
+      <c r="AA28" s="3"/>
+      <c r="AB28" s="3"/>
+      <c r="AC28" s="3"/>
+      <c r="AD28" s="3"/>
+      <c r="AE28" s="3"/>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
       <c r="D29" s="1">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
       <c r="J29" s="1">
         <f t="shared" si="4"/>
         <v>28</v>
       </c>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
       <c r="P29" s="1">
         <f t="shared" si="7"/>
         <v>28</v>
@@ -1824,16 +2296,37 @@
         <f t="shared" si="9"/>
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="V29" s="3"/>
+      <c r="W29" s="3"/>
+      <c r="X29" s="3"/>
+      <c r="Y29" s="3"/>
+      <c r="Z29" s="3"/>
+      <c r="AA29" s="3"/>
+      <c r="AB29" s="3"/>
+      <c r="AC29" s="3"/>
+      <c r="AD29" s="3"/>
+      <c r="AE29" s="3"/>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
       <c r="D30" s="1">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
       <c r="J30" s="1">
         <f t="shared" si="4"/>
         <v>29</v>
       </c>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
       <c r="P30" s="1">
         <f t="shared" si="7"/>
         <v>29</v>
@@ -1846,12 +2339,35 @@
         <f t="shared" si="9"/>
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="V30" s="3"/>
+      <c r="W30" s="3"/>
+      <c r="X30" s="3"/>
+      <c r="Y30" s="3"/>
+      <c r="Z30" s="3"/>
+      <c r="AA30" s="3"/>
+      <c r="AB30" s="3"/>
+      <c r="AC30" s="3"/>
+      <c r="AD30" s="3"/>
+      <c r="AE30" s="3"/>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
       <c r="D31" s="1">
         <f>D30+1</f>
         <v>30</v>
       </c>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
       <c r="P31" s="1">
         <f t="shared" si="7"/>
         <v>30</v>
@@ -1864,8 +2380,33 @@
         <f t="shared" si="9"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="V31" s="3"/>
+      <c r="W31" s="3"/>
+      <c r="X31" s="3"/>
+      <c r="Y31" s="3"/>
+      <c r="Z31" s="3"/>
+      <c r="AA31" s="3"/>
+      <c r="AB31" s="3"/>
+      <c r="AC31" s="3"/>
+      <c r="AD31" s="3"/>
+      <c r="AE31" s="3"/>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
       <c r="P32" s="1">
         <f t="shared" si="7"/>
         <v>31</v>
@@ -1878,69 +2419,158 @@
         <f t="shared" si="9"/>
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V32" s="3"/>
+      <c r="W32" s="3"/>
+      <c r="X32" s="3"/>
+      <c r="Y32" s="3"/>
+      <c r="Z32" s="3"/>
+      <c r="AA32" s="3"/>
+      <c r="AB32" s="3"/>
+      <c r="AC32" s="3"/>
+      <c r="AD32" s="3"/>
+      <c r="AE32" s="3"/>
+    </row>
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="3"/>
       <c r="T33" s="1">
         <f t="shared" si="9"/>
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="C35" s="1" t="str">
+      <c r="V33" s="3"/>
+      <c r="W33" s="3"/>
+      <c r="X33" s="3"/>
+      <c r="Y33" s="3"/>
+      <c r="Z33" s="3"/>
+      <c r="AA33" s="3"/>
+      <c r="AB33" s="3"/>
+      <c r="AC33" s="3"/>
+      <c r="AD33" s="3"/>
+      <c r="AE33" s="3"/>
+    </row>
+    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="3"/>
+      <c r="T34" s="3"/>
+      <c r="U34" s="3"/>
+      <c r="V34" s="3"/>
+      <c r="W34" s="3"/>
+      <c r="X34" s="3"/>
+      <c r="Y34" s="3"/>
+      <c r="Z34" s="3"/>
+      <c r="AA34" s="3"/>
+      <c r="AB34" s="3"/>
+      <c r="AC34" s="3"/>
+      <c r="AD34" s="3"/>
+      <c r="AE34" s="3"/>
+    </row>
+    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="C35" s="6" t="str">
         <f>B$1</f>
         <v>Chapter 1</v>
       </c>
-      <c r="E35" s="1" t="str">
+      <c r="D35" s="6"/>
+      <c r="E35" s="6" t="str">
         <f t="shared" ref="D35:W35" si="11">D$1</f>
         <v>Chapter 2</v>
       </c>
-      <c r="G35" s="1" t="str">
+      <c r="F35" s="6"/>
+      <c r="G35" s="6" t="str">
         <f t="shared" si="11"/>
         <v>Chapter 3</v>
       </c>
-      <c r="I35" s="1" t="str">
+      <c r="H35" s="6"/>
+      <c r="I35" s="6" t="str">
         <f t="shared" si="11"/>
         <v>Chapter 4</v>
       </c>
-      <c r="K35" s="1" t="str">
+      <c r="J35" s="6"/>
+      <c r="K35" s="6" t="str">
         <f t="shared" si="11"/>
         <v>Chapter 5</v>
       </c>
-      <c r="M35" s="1" t="str">
+      <c r="L35" s="6"/>
+      <c r="M35" s="6" t="str">
         <f t="shared" si="11"/>
         <v>Chapter 6</v>
       </c>
-      <c r="O35" s="1" t="str">
+      <c r="N35" s="6"/>
+      <c r="O35" s="6" t="str">
         <f t="shared" si="11"/>
         <v>Chapter 7</v>
       </c>
-      <c r="Q35" s="1" t="str">
+      <c r="P35" s="6"/>
+      <c r="Q35" s="6" t="str">
         <f t="shared" si="11"/>
         <v>Chapter 8</v>
       </c>
-      <c r="S35" s="1" t="str">
+      <c r="R35" s="6"/>
+      <c r="S35" s="6" t="str">
         <f t="shared" si="11"/>
         <v>Chapter 9</v>
       </c>
-      <c r="U35" s="1" t="str">
+      <c r="T35" s="6"/>
+      <c r="U35" s="6" t="str">
         <f t="shared" si="11"/>
         <v>Chapter 10</v>
       </c>
-      <c r="W35" s="1" t="str">
+      <c r="V35" s="6"/>
+      <c r="W35" s="6" t="str">
         <f t="shared" si="11"/>
         <v>Chapter 11</v>
       </c>
-      <c r="Y35" s="1" t="s">
+      <c r="X35" s="6"/>
+      <c r="Y35" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z35" s="3"/>
+      <c r="AA35" s="3"/>
+      <c r="AB35" s="3"/>
+      <c r="AC35" s="3"/>
+      <c r="AD35" s="3"/>
+      <c r="AE35" s="3"/>
+    </row>
+    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C36" s="1">
         <f>COUNTIF(C$2:C$33,"In Progress")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E36" s="1">
         <f t="shared" ref="E36:W36" si="12">COUNTIF(E$2:E$33,"In Progress")</f>
@@ -1987,10 +2617,16 @@
       </c>
       <c r="Y36" s="1">
         <f>SUM(C36:W36)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="Z36" s="3"/>
+      <c r="AA36" s="3"/>
+      <c r="AB36" s="3"/>
+      <c r="AC36" s="3"/>
+      <c r="AD36" s="3"/>
+      <c r="AE36" s="3"/>
+    </row>
+    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>2</v>
       </c>
@@ -2045,8 +2681,14 @@
         <f t="shared" ref="Y37:Y38" si="14">SUM(C37:W37)</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z37" s="3"/>
+      <c r="AA37" s="3"/>
+      <c r="AB37" s="3"/>
+      <c r="AC37" s="3"/>
+      <c r="AD37" s="3"/>
+      <c r="AE37" s="3"/>
+    </row>
+    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>15</v>
       </c>
@@ -2101,63 +2743,319 @@
         <f t="shared" si="14"/>
         <v>287</v>
       </c>
-    </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z38" s="3"/>
+      <c r="AA38" s="3"/>
+      <c r="AB38" s="3"/>
+      <c r="AC38" s="3"/>
+      <c r="AD38" s="3"/>
+      <c r="AE38" s="3"/>
+    </row>
+    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C39" s="2">
         <f>C$37/C$38</f>
         <v>0.3</v>
       </c>
-      <c r="E39" s="3">
+      <c r="E39" s="2">
         <f>E$37/E$38</f>
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="G39" s="3">
+      <c r="G39" s="2">
         <f>G$37/G$38</f>
         <v>0.04</v>
       </c>
-      <c r="I39" s="3">
+      <c r="I39" s="2">
         <f>I$37/I$38</f>
         <v>0</v>
       </c>
-      <c r="K39" s="3">
+      <c r="K39" s="2">
         <f>K$37/K$38</f>
         <v>3.4482758620689655E-2</v>
       </c>
-      <c r="M39" s="3">
+      <c r="M39" s="2">
         <f>M$37/M$38</f>
         <v>0</v>
       </c>
-      <c r="O39" s="3">
+      <c r="O39" s="2">
         <f>O$37/O$38</f>
         <v>0</v>
       </c>
-      <c r="Q39" s="3">
+      <c r="Q39" s="2">
         <f>Q$37/Q$38</f>
         <v>0</v>
       </c>
-      <c r="S39" s="3">
+      <c r="S39" s="2">
         <f>S$37/S$38</f>
         <v>0</v>
       </c>
-      <c r="U39" s="3">
+      <c r="U39" s="2">
         <f>U$37/U$38</f>
         <v>0</v>
       </c>
-      <c r="W39" s="3">
+      <c r="W39" s="2">
         <f>W$37/W$38</f>
         <v>0</v>
       </c>
       <c r="X39" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Y39" s="3">
+      <c r="Y39" s="2">
         <f>Y37/Y38</f>
         <v>3.484320557491289E-2</v>
       </c>
-    </row>
+      <c r="Z39" s="3"/>
+      <c r="AA39" s="3"/>
+      <c r="AB39" s="3"/>
+      <c r="AC39" s="3"/>
+      <c r="AD39" s="3"/>
+      <c r="AE39" s="3"/>
+    </row>
+    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
+      <c r="O40" s="3"/>
+      <c r="P40" s="3"/>
+      <c r="Q40" s="3"/>
+      <c r="R40" s="3"/>
+      <c r="S40" s="3"/>
+      <c r="T40" s="3"/>
+      <c r="U40" s="3"/>
+      <c r="V40" s="3"/>
+      <c r="W40" s="3"/>
+      <c r="X40" s="3"/>
+      <c r="Y40" s="3"/>
+      <c r="Z40" s="3"/>
+      <c r="AA40" s="3"/>
+      <c r="AB40" s="3"/>
+      <c r="AC40" s="3"/>
+      <c r="AD40" s="3"/>
+      <c r="AE40" s="3"/>
+    </row>
+    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
+      <c r="O41" s="3"/>
+      <c r="P41" s="3"/>
+      <c r="Q41" s="3"/>
+      <c r="R41" s="3"/>
+      <c r="S41" s="3"/>
+      <c r="T41" s="3"/>
+      <c r="U41" s="3"/>
+      <c r="V41" s="3"/>
+      <c r="W41" s="3"/>
+      <c r="X41" s="3"/>
+      <c r="Y41" s="3"/>
+      <c r="Z41" s="3"/>
+      <c r="AA41" s="3"/>
+      <c r="AB41" s="3"/>
+      <c r="AC41" s="3"/>
+      <c r="AD41" s="3"/>
+      <c r="AE41" s="3"/>
+    </row>
+    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3"/>
+      <c r="N42" s="3"/>
+      <c r="O42" s="3"/>
+      <c r="P42" s="3"/>
+      <c r="Q42" s="3"/>
+      <c r="R42" s="3"/>
+      <c r="S42" s="3"/>
+      <c r="T42" s="3"/>
+      <c r="U42" s="3"/>
+      <c r="V42" s="3"/>
+      <c r="W42" s="3"/>
+      <c r="X42" s="3"/>
+      <c r="Y42" s="3"/>
+      <c r="Z42" s="3"/>
+      <c r="AA42" s="3"/>
+      <c r="AB42" s="3"/>
+      <c r="AC42" s="3"/>
+      <c r="AD42" s="3"/>
+      <c r="AE42" s="3"/>
+    </row>
+    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
+      <c r="O43" s="3"/>
+      <c r="P43" s="3"/>
+      <c r="Q43" s="3"/>
+      <c r="R43" s="3"/>
+      <c r="S43" s="3"/>
+      <c r="T43" s="3"/>
+      <c r="U43" s="3"/>
+      <c r="V43" s="3"/>
+      <c r="W43" s="3"/>
+      <c r="X43" s="3"/>
+      <c r="Y43" s="3"/>
+      <c r="Z43" s="3"/>
+      <c r="AA43" s="3"/>
+      <c r="AB43" s="3"/>
+      <c r="AC43" s="3"/>
+      <c r="AD43" s="3"/>
+      <c r="AE43" s="3"/>
+    </row>
+    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="3"/>
+      <c r="N44" s="3"/>
+      <c r="O44" s="3"/>
+      <c r="P44" s="3"/>
+      <c r="Q44" s="3"/>
+      <c r="R44" s="3"/>
+      <c r="S44" s="3"/>
+      <c r="T44" s="3"/>
+      <c r="U44" s="3"/>
+      <c r="V44" s="3"/>
+      <c r="W44" s="3"/>
+      <c r="X44" s="3"/>
+      <c r="Y44" s="3"/>
+      <c r="Z44" s="3"/>
+      <c r="AA44" s="3"/>
+      <c r="AB44" s="3"/>
+      <c r="AC44" s="3"/>
+      <c r="AD44" s="3"/>
+      <c r="AE44" s="3"/>
+    </row>
+    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="3"/>
+      <c r="O45" s="3"/>
+      <c r="P45" s="3"/>
+      <c r="Q45" s="3"/>
+      <c r="R45" s="3"/>
+      <c r="S45" s="3"/>
+      <c r="T45" s="3"/>
+      <c r="U45" s="3"/>
+      <c r="V45" s="3"/>
+      <c r="W45" s="3"/>
+      <c r="X45" s="3"/>
+      <c r="Y45" s="3"/>
+      <c r="Z45" s="3"/>
+      <c r="AA45" s="3"/>
+      <c r="AB45" s="3"/>
+      <c r="AC45" s="3"/>
+      <c r="AD45" s="3"/>
+      <c r="AE45" s="3"/>
+    </row>
+    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
+      <c r="M46" s="3"/>
+      <c r="N46" s="3"/>
+      <c r="O46" s="3"/>
+      <c r="P46" s="3"/>
+      <c r="Q46" s="3"/>
+      <c r="R46" s="3"/>
+      <c r="S46" s="3"/>
+      <c r="T46" s="3"/>
+      <c r="U46" s="3"/>
+      <c r="V46" s="3"/>
+      <c r="W46" s="3"/>
+      <c r="X46" s="3"/>
+      <c r="Y46" s="3"/>
+      <c r="Z46" s="3"/>
+      <c r="AA46" s="3"/>
+      <c r="AB46" s="3"/>
+      <c r="AC46" s="3"/>
+      <c r="AD46" s="3"/>
+      <c r="AE46" s="3"/>
+    </row>
+    <row r="47" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="N1:O1"/>
@@ -2177,24 +3075,24 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{3E9AD461-33FE-4C12-BC5D-6843F8759F43}">
+          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{403F3712-C03D-4299-8025-B7221537FEE1}">
             <xm:f>NOT(ISERROR(SEARCH(Sheet2!$A$3,C2)))</xm:f>
             <xm:f>Sheet2!$A$3</xm:f>
             <x14:dxf>
               <font>
                 <strike val="0"/>
-                <color theme="0"/>
+                <color theme="0" tint="-4.9989318521683403E-2"/>
               </font>
               <fill>
                 <patternFill>
-                  <bgColor rgb="FFFEEC00"/>
+                  <bgColor rgb="FFCC0000"/>
                 </patternFill>
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{83F44093-A430-4148-9498-2DA9893DB6C7}">
-            <xm:f>NOT(ISERROR(SEARCH(Sheet2!$A$4,C2)))</xm:f>
-            <xm:f>Sheet2!$A$4</xm:f>
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{83F44093-A430-4148-9498-2DA9893DB6C7}">
+            <xm:f>NOT(ISERROR(SEARCH(Sheet2!$A$5,C2)))</xm:f>
+            <xm:f>Sheet2!$A$5</xm:f>
             <x14:dxf>
               <font>
                 <strike val="0"/>
@@ -2209,15 +3107,33 @@
           </x14:cfRule>
           <xm:sqref>E2:E31 G2:G26 I2:I27 C2:C21 K2:K30 M2:M20 O2:O27 Q2:Q32 S2:S32 U2:U34 W2:W19 U36</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{C3C15BD9-8F3C-462A-967D-DE84A0677643}">
+            <xm:f>NOT(ISERROR(SEARCH(Sheet2!$A$4,C2)))</xm:f>
+            <xm:f>Sheet2!$A$4</xm:f>
+            <x14:dxf>
+              <font>
+                <strike val="0"/>
+                <color theme="0" tint="-0.34998626667073579"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFF30D"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>E2:E31 G2:G26 I2:I27 C2:C21 K2:K30 M2:M20 O2:O27 Q2:Q32 S2:S32 U2:U33 W2:W19</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{E699E494-36BB-4C22-9D71-A8DC2FECC4EE}">
           <x14:formula1>
-            <xm:f>Sheet2!$A$2:$A$4</xm:f>
+            <xm:f>Sheet2!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E31 G2:G26 I2:I27 C2:C21 K2:K30 M2:M20 O2:O27 Q2:Q32 S2:S32 W2:W19 U2:U34 U36</xm:sqref>
+          <xm:sqref>E2:E31 U36 U2:U34 W2:W19 S2:S32 Q2:Q32 O2:O27 M2:M20 K2:K30 C2:C21 I2:I27 G2:G26</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2227,15 +3143,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3B5FE83-5048-4F6C-8894-3FCD7FD7BA73}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -2251,6 +3167,11 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>